<commit_message>
Added PDF's and modified xlsx file
</commit_message>
<xml_diff>
--- a/otherinfos/Kalibration/DruckSensor (version 1).xlsx
+++ b/otherinfos/Kalibration/DruckSensor (version 1).xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D5A4F6F-7251-46DD-A90D-F91E5789D89D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5999D909-CE3B-401B-AAA9-C4D92A180905}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Infos" sheetId="10" r:id="rId1"/>
@@ -15,9 +15,9 @@
     <sheet name="Analog" sheetId="4" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'P1 Spannung'!$B$2:$J$8</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">'P2 Spannung'!$B$2:$J$8</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="3">'P3 Spannung'!$B$2:$J$8</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'P1 Spannung'!$A:$R</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">'P2 Spannung'!$A:$R</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">'P3 Spannung'!$A:$R</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -873,18 +873,6 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -895,15 +883,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -911,15 +890,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -928,15 +898,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -983,6 +944,45 @@
     <xf numFmtId="2" fontId="0" fillId="3" borderId="33" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="3" borderId="28" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -21038,15 +21038,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>7140</xdr:colOff>
+      <xdr:colOff>23015</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>202404</xdr:rowOff>
+      <xdr:rowOff>186529</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>-1</xdr:colOff>
+      <xdr:colOff>15874</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>345281</xdr:rowOff>
+      <xdr:rowOff>329406</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -21888,7 +21888,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F616FF6-8926-4223-AA20-EFFB0EBBC2D2}">
   <dimension ref="B1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
@@ -21900,20 +21900,20 @@
   <sheetData>
     <row r="1" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="79" t="s">
+      <c r="B2" s="101" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="80"/>
-      <c r="D2" s="81"/>
+      <c r="C2" s="102"/>
+      <c r="D2" s="103"/>
     </row>
     <row r="3" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="82" t="s">
+      <c r="B3" s="75" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="82" t="s">
+      <c r="C3" s="75" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="82" t="s">
+      <c r="D3" s="75" t="s">
         <v>45</v>
       </c>
     </row>
@@ -21921,26 +21921,26 @@
       <c r="B4" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="77">
+      <c r="C4" s="73">
         <v>1</v>
       </c>
-      <c r="D4" s="77" t="s">
+      <c r="D4" s="73" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="5" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="83" t="s">
+      <c r="B5" s="76" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="84">
+      <c r="C5" s="77">
         <v>0.01</v>
       </c>
-      <c r="D5" s="84" t="s">
+      <c r="D5" s="77" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="6" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="78" t="s">
+      <c r="B6" s="74" t="s">
         <v>48</v>
       </c>
       <c r="C6" s="64">
@@ -21955,6 +21955,7 @@
     <mergeCell ref="B2:D2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -21962,8 +21963,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82D6FC5D-20FD-4585-85D2-0A365BB12AD8}">
   <dimension ref="B1:AA40"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39:I39"/>
+    <sheetView view="pageBreakPreview" zoomScale="60" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="Y11" sqref="Y11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21978,60 +21979,60 @@
     <col min="8" max="8" width="18.7109375" customWidth="1"/>
     <col min="9" max="9" width="13.85546875" customWidth="1"/>
     <col min="10" max="10" width="21.28515625" customWidth="1"/>
-    <col min="11" max="11" width="17.85546875" customWidth="1"/>
+    <col min="11" max="11" width="7.85546875" customWidth="1"/>
     <col min="12" max="12" width="17.5703125" customWidth="1"/>
     <col min="13" max="13" width="19.140625" customWidth="1"/>
     <col min="14" max="14" width="19.28515625" customWidth="1"/>
     <col min="15" max="15" width="19" customWidth="1"/>
     <col min="16" max="16" width="22" customWidth="1"/>
     <col min="17" max="17" width="23.28515625" customWidth="1"/>
-    <col min="18" max="18" width="20.28515625" customWidth="1"/>
+    <col min="18" max="18" width="12" customWidth="1"/>
     <col min="19" max="19" width="29.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="85" t="s">
+      <c r="B2" s="105" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="86"/>
-      <c r="I2" s="86"/>
-      <c r="J2" s="87"/>
+      <c r="C2" s="106"/>
+      <c r="D2" s="106"/>
+      <c r="E2" s="106"/>
+      <c r="F2" s="106"/>
+      <c r="G2" s="106"/>
+      <c r="H2" s="106"/>
+      <c r="I2" s="106"/>
+      <c r="J2" s="107"/>
       <c r="S2" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="3" spans="2:27" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="88" t="s">
+      <c r="B3" s="78" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="88" t="s">
+      <c r="C3" s="78" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="88" t="s">
+      <c r="D3" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="88" t="s">
+      <c r="E3" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="89" t="s">
+      <c r="F3" s="79" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="88" t="s">
+      <c r="G3" s="78" t="s">
         <v>39</v>
       </c>
-      <c r="H3" s="88" t="s">
+      <c r="H3" s="78" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="90" t="s">
+      <c r="I3" s="80" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="89" t="s">
+      <c r="J3" s="79" t="s">
         <v>16</v>
       </c>
       <c r="L3" s="26"/>
@@ -22087,31 +22088,31 @@
       <c r="S4" s="36"/>
     </row>
     <row r="5" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="98">
+      <c r="B5" s="85">
         <v>80</v>
       </c>
-      <c r="C5" s="99">
+      <c r="C5" s="86">
         <v>20.010000000000002</v>
       </c>
-      <c r="D5" s="100">
+      <c r="D5" s="87">
         <v>19.84</v>
       </c>
-      <c r="E5" s="101">
+      <c r="E5" s="88">
         <v>20</v>
       </c>
-      <c r="F5" s="102">
+      <c r="F5" s="89">
         <f t="shared" ref="F5:F8" si="0">(C5+D5+E5)/3</f>
         <v>19.95</v>
       </c>
-      <c r="G5" s="103">
+      <c r="G5" s="90">
         <f t="shared" ref="G5:G8" si="1">MAX(C5-F5,D5-F5,E5-F5)*$S$3</f>
         <v>6.0000000000002274E-2</v>
       </c>
-      <c r="H5" s="104">
+      <c r="H5" s="91">
         <f t="shared" ref="H5:H8" si="2">(G5/$S$3)/(MAX($C$4:$E$8)-MIN($C$4:$E$8))</f>
         <v>1.0467550593161597E-3</v>
       </c>
-      <c r="I5" s="97" t="s">
+      <c r="I5" s="84" t="s">
         <v>38</v>
       </c>
       <c r="J5" s="47"/>
@@ -22162,27 +22163,27 @@
       <c r="S6" s="36"/>
     </row>
     <row r="7" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B7" s="98">
+      <c r="B7" s="85">
         <v>240</v>
       </c>
-      <c r="C7" s="99">
+      <c r="C7" s="86">
         <v>51.1</v>
       </c>
-      <c r="D7" s="100">
+      <c r="D7" s="87">
         <v>51.3</v>
       </c>
-      <c r="E7" s="101">
+      <c r="E7" s="88">
         <v>51.23</v>
       </c>
-      <c r="F7" s="102">
+      <c r="F7" s="89">
         <f t="shared" si="0"/>
         <v>51.21</v>
       </c>
-      <c r="G7" s="103">
+      <c r="G7" s="90">
         <f t="shared" si="1"/>
         <v>8.9999999999996305E-2</v>
       </c>
-      <c r="H7" s="104">
+      <c r="H7" s="91">
         <f t="shared" si="2"/>
         <v>1.5701325889741155E-3</v>
       </c>
@@ -22240,47 +22241,47 @@
       <c r="I9" s="36"/>
     </row>
     <row r="10" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="85" t="s">
+      <c r="B10" s="105" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="86"/>
-      <c r="D10" s="86"/>
-      <c r="E10" s="86"/>
-      <c r="F10" s="86"/>
-      <c r="G10" s="86"/>
-      <c r="H10" s="86"/>
-      <c r="I10" s="86"/>
-      <c r="J10" s="87"/>
-      <c r="Y10" s="67"/>
-      <c r="Z10" s="67"/>
-      <c r="AA10" s="67"/>
+      <c r="C10" s="106"/>
+      <c r="D10" s="106"/>
+      <c r="E10" s="106"/>
+      <c r="F10" s="106"/>
+      <c r="G10" s="106"/>
+      <c r="H10" s="106"/>
+      <c r="I10" s="106"/>
+      <c r="J10" s="107"/>
+      <c r="Y10" s="104"/>
+      <c r="Z10" s="104"/>
+      <c r="AA10" s="104"/>
     </row>
     <row r="11" spans="2:27" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="88" t="s">
+      <c r="B11" s="78" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="88" t="s">
+      <c r="C11" s="78" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="88" t="s">
+      <c r="D11" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="88" t="s">
+      <c r="E11" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="F11" s="89" t="s">
+      <c r="F11" s="79" t="s">
         <v>21</v>
       </c>
-      <c r="G11" s="88" t="s">
+      <c r="G11" s="78" t="s">
         <v>39</v>
       </c>
-      <c r="H11" s="88" t="s">
+      <c r="H11" s="78" t="s">
         <v>22</v>
       </c>
-      <c r="I11" s="90" t="s">
+      <c r="I11" s="80" t="s">
         <v>23</v>
       </c>
-      <c r="J11" s="89" t="s">
+      <c r="J11" s="79" t="s">
         <v>16</v>
       </c>
     </row>
@@ -22320,27 +22321,27 @@
       <c r="K12" s="34"/>
     </row>
     <row r="13" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B13" s="98">
+      <c r="B13" s="85">
         <v>80</v>
       </c>
-      <c r="C13" s="100">
+      <c r="C13" s="87">
         <v>23.23</v>
       </c>
-      <c r="D13" s="100">
+      <c r="D13" s="87">
         <v>23.2</v>
       </c>
-      <c r="E13" s="100">
+      <c r="E13" s="87">
         <v>23.41</v>
       </c>
-      <c r="F13" s="102">
+      <c r="F13" s="89">
         <f t="shared" ref="F13:F16" si="3">(C13+D13+E13)/3</f>
         <v>23.28</v>
       </c>
-      <c r="G13" s="103">
+      <c r="G13" s="90">
         <f t="shared" ref="G13:G16" si="4">MAX(C13-F13,D13-F13,E13-F13)*$S$3</f>
         <v>0.12999999999999901</v>
       </c>
-      <c r="H13" s="104">
+      <c r="H13" s="91">
         <f t="shared" ref="H13:H16" si="5">(G13/$S$3)/(MAX($C$12:$E$16)-MIN($C$12:$E$16))</f>
         <v>1.9374068554396276E-3</v>
       </c>
@@ -22374,27 +22375,27 @@
       <c r="J14" s="47"/>
     </row>
     <row r="15" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B15" s="98">
+      <c r="B15" s="85">
         <v>240</v>
       </c>
-      <c r="C15" s="100">
+      <c r="C15" s="87">
         <v>60.13</v>
       </c>
-      <c r="D15" s="100">
+      <c r="D15" s="87">
         <v>60.27</v>
       </c>
-      <c r="E15" s="100">
+      <c r="E15" s="87">
         <v>59.78</v>
       </c>
-      <c r="F15" s="102">
+      <c r="F15" s="89">
         <f t="shared" si="3"/>
         <v>60.06</v>
       </c>
-      <c r="G15" s="103">
+      <c r="G15" s="90">
         <f t="shared" si="4"/>
         <v>0.21000000000000085</v>
       </c>
-      <c r="H15" s="104">
+      <c r="H15" s="91">
         <f t="shared" si="5"/>
         <v>3.1296572280178968E-3</v>
       </c>
@@ -22430,44 +22431,44 @@
     </row>
     <row r="17" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="18" spans="2:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="91" t="s">
+      <c r="B18" s="108" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="92"/>
-      <c r="D18" s="92"/>
-      <c r="E18" s="92"/>
-      <c r="F18" s="92"/>
-      <c r="G18" s="92"/>
-      <c r="H18" s="92"/>
-      <c r="I18" s="92"/>
-      <c r="J18" s="93"/>
+      <c r="C18" s="109"/>
+      <c r="D18" s="109"/>
+      <c r="E18" s="109"/>
+      <c r="F18" s="109"/>
+      <c r="G18" s="109"/>
+      <c r="H18" s="109"/>
+      <c r="I18" s="109"/>
+      <c r="J18" s="110"/>
     </row>
     <row r="19" spans="2:15" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="94" t="s">
+      <c r="B19" s="81" t="s">
         <v>34</v>
       </c>
-      <c r="C19" s="95" t="s">
+      <c r="C19" s="82" t="s">
         <v>31</v>
       </c>
-      <c r="D19" s="95" t="s">
+      <c r="D19" s="82" t="s">
         <v>32</v>
       </c>
-      <c r="E19" s="95" t="s">
+      <c r="E19" s="82" t="s">
         <v>33</v>
       </c>
-      <c r="F19" s="90" t="s">
+      <c r="F19" s="80" t="s">
         <v>21</v>
       </c>
-      <c r="G19" s="95" t="s">
+      <c r="G19" s="82" t="s">
         <v>39</v>
       </c>
-      <c r="H19" s="95" t="s">
+      <c r="H19" s="82" t="s">
         <v>22</v>
       </c>
-      <c r="I19" s="96" t="s">
+      <c r="I19" s="83" t="s">
         <v>24</v>
       </c>
-      <c r="J19" s="95" t="s">
+      <c r="J19" s="82" t="s">
         <v>40</v>
       </c>
     </row>
@@ -22498,7 +22499,7 @@
         <f>(G20)/((MAX($C$20:$E$24)-MIN($C$20:$E$24)))</f>
         <v>2.2055836090312891E-3</v>
       </c>
-      <c r="I20" s="74">
+      <c r="I20" s="70">
         <f>F20-B20</f>
         <v>0.10333333333333306</v>
       </c>
@@ -22508,31 +22509,31 @@
       </c>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B21" s="103">
+      <c r="B21" s="90">
         <v>19.95</v>
       </c>
-      <c r="C21" s="105">
+      <c r="C21" s="92">
         <v>19.760000000000002</v>
       </c>
-      <c r="D21" s="106">
+      <c r="D21" s="93">
         <v>19.71</v>
       </c>
-      <c r="E21" s="107">
+      <c r="E21" s="94">
         <v>19.8</v>
       </c>
-      <c r="F21" s="102">
+      <c r="F21" s="89">
         <f t="shared" ref="F21:F24" si="6">(C21+D21+E21)/3</f>
         <v>19.756666666666664</v>
       </c>
-      <c r="G21" s="103">
+      <c r="G21" s="90">
         <f t="shared" ref="G21:G24" si="7">MAX(C21-F21,D21-F21,E21-F21)*$S$3</f>
         <v>4.3333333333336554E-2</v>
       </c>
-      <c r="H21" s="104">
+      <c r="H21" s="91">
         <f t="shared" ref="H21:H23" si="8">(G21)/((MAX($C$20:$E$24)-MIN($C$20:$E$24)))</f>
         <v>7.5454176098444284E-4</v>
       </c>
-      <c r="I21" s="108">
+      <c r="I21" s="95">
         <f t="shared" ref="I21:I24" si="9">F21-B21</f>
         <v>-0.19333333333333513</v>
       </c>
@@ -22564,7 +22565,7 @@
         <f t="shared" si="8"/>
         <v>9.8670845667185917E-4</v>
       </c>
-      <c r="I22" s="75">
+      <c r="I22" s="71">
         <f t="shared" si="9"/>
         <v>9.0000000000003411E-2</v>
       </c>
@@ -22572,31 +22573,31 @@
       <c r="L22" s="2"/>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B23" s="103">
+      <c r="B23" s="90">
         <v>51.21</v>
       </c>
-      <c r="C23" s="105">
+      <c r="C23" s="92">
         <v>51.3</v>
       </c>
-      <c r="D23" s="106">
+      <c r="D23" s="93">
         <v>51.5</v>
       </c>
-      <c r="E23" s="107">
+      <c r="E23" s="94">
         <v>51.46</v>
       </c>
-      <c r="F23" s="102">
+      <c r="F23" s="89">
         <f t="shared" si="6"/>
         <v>51.419999999999995</v>
       </c>
-      <c r="G23" s="103">
+      <c r="G23" s="90">
         <f t="shared" si="7"/>
         <v>8.00000000000054E-2</v>
       </c>
-      <c r="H23" s="104">
+      <c r="H23" s="91">
         <f t="shared" si="8"/>
         <v>1.3930001741251157E-3</v>
       </c>
-      <c r="I23" s="108">
+      <c r="I23" s="95">
         <f t="shared" si="9"/>
         <v>0.20999999999999375</v>
       </c>
@@ -22628,7 +22629,7 @@
         <f>(G24)/((MAX($C$20:$E$24)-MIN($C$20:$E$24)))</f>
         <v>2.0895002611874881E-3</v>
       </c>
-      <c r="I24" s="76">
+      <c r="I24" s="72">
         <f t="shared" si="9"/>
         <v>-3.3333333333303017E-3</v>
       </c>
@@ -22639,45 +22640,45 @@
       <c r="L25" s="2"/>
     </row>
     <row r="26" spans="2:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="85" t="s">
+      <c r="B26" s="105" t="s">
         <v>35</v>
       </c>
-      <c r="C26" s="86"/>
-      <c r="D26" s="86"/>
-      <c r="E26" s="86"/>
-      <c r="F26" s="86"/>
-      <c r="G26" s="86"/>
-      <c r="H26" s="86"/>
-      <c r="I26" s="86"/>
-      <c r="J26" s="87"/>
+      <c r="C26" s="106"/>
+      <c r="D26" s="106"/>
+      <c r="E26" s="106"/>
+      <c r="F26" s="106"/>
+      <c r="G26" s="106"/>
+      <c r="H26" s="106"/>
+      <c r="I26" s="106"/>
+      <c r="J26" s="107"/>
       <c r="L26" s="2"/>
     </row>
     <row r="27" spans="2:15" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="88" t="s">
+      <c r="B27" s="78" t="s">
         <v>15</v>
       </c>
-      <c r="C27" s="88" t="s">
+      <c r="C27" s="78" t="s">
         <v>12</v>
       </c>
-      <c r="D27" s="88" t="s">
+      <c r="D27" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="E27" s="88" t="s">
+      <c r="E27" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="F27" s="89" t="s">
+      <c r="F27" s="79" t="s">
         <v>21</v>
       </c>
-      <c r="G27" s="88" t="s">
+      <c r="G27" s="78" t="s">
         <v>39</v>
       </c>
-      <c r="H27" s="88" t="s">
+      <c r="H27" s="78" t="s">
         <v>22</v>
       </c>
-      <c r="I27" s="90" t="s">
+      <c r="I27" s="80" t="s">
         <v>23</v>
       </c>
-      <c r="J27" s="89" t="s">
+      <c r="J27" s="79" t="s">
         <v>16</v>
       </c>
       <c r="L27" s="2"/>
@@ -22718,27 +22719,27 @@
       <c r="L28" s="2"/>
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B29" s="98">
+      <c r="B29" s="85">
         <v>80</v>
       </c>
-      <c r="C29" s="100">
+      <c r="C29" s="87">
         <v>19.760000000000002</v>
       </c>
-      <c r="D29" s="100">
+      <c r="D29" s="87">
         <v>19.71</v>
       </c>
-      <c r="E29" s="100">
+      <c r="E29" s="87">
         <v>19.8</v>
       </c>
-      <c r="F29" s="102">
+      <c r="F29" s="89">
         <f t="shared" ref="F29:F32" si="10">(C29+D29+E29)/3</f>
         <v>19.756666666666664</v>
       </c>
-      <c r="G29" s="103">
+      <c r="G29" s="90">
         <f t="shared" ref="G29:G32" si="11">MAX(C29-F29,D29-F29,E29-F29)*$S$3</f>
         <v>4.3333333333336554E-2</v>
       </c>
-      <c r="H29" s="104">
+      <c r="H29" s="91">
         <f t="shared" ref="H29:H32" si="12">(G29/$S$3)/(MAX($C$28:$E$32)-MIN($C$28:$E$32))</f>
         <v>7.5454176098444284E-4</v>
       </c>
@@ -22778,27 +22779,27 @@
       <c r="O30" s="42"/>
     </row>
     <row r="31" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B31" s="98">
+      <c r="B31" s="85">
         <v>240</v>
       </c>
-      <c r="C31" s="100">
+      <c r="C31" s="87">
         <v>51.3</v>
       </c>
-      <c r="D31" s="100">
+      <c r="D31" s="87">
         <v>51.5</v>
       </c>
-      <c r="E31" s="100">
+      <c r="E31" s="87">
         <v>51.46</v>
       </c>
-      <c r="F31" s="102">
+      <c r="F31" s="89">
         <f t="shared" si="10"/>
         <v>51.419999999999995</v>
       </c>
-      <c r="G31" s="103">
+      <c r="G31" s="90">
         <f t="shared" si="11"/>
         <v>8.00000000000054E-2</v>
       </c>
-      <c r="H31" s="104">
+      <c r="H31" s="91">
         <f t="shared" si="12"/>
         <v>1.3930001741251157E-3</v>
       </c>
@@ -22837,44 +22838,44 @@
       <c r="G33"/>
     </row>
     <row r="34" spans="2:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="91" t="s">
+      <c r="B34" s="108" t="s">
         <v>25</v>
       </c>
-      <c r="C34" s="92"/>
-      <c r="D34" s="92"/>
-      <c r="E34" s="92"/>
-      <c r="F34" s="92"/>
-      <c r="G34" s="92"/>
-      <c r="H34" s="92"/>
-      <c r="I34" s="92"/>
-      <c r="J34" s="93"/>
+      <c r="C34" s="109"/>
+      <c r="D34" s="109"/>
+      <c r="E34" s="109"/>
+      <c r="F34" s="109"/>
+      <c r="G34" s="109"/>
+      <c r="H34" s="109"/>
+      <c r="I34" s="109"/>
+      <c r="J34" s="110"/>
     </row>
     <row r="35" spans="2:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="94" t="s">
+      <c r="B35" s="81" t="s">
         <v>15</v>
       </c>
-      <c r="C35" s="95" t="s">
+      <c r="C35" s="82" t="s">
         <v>26</v>
       </c>
-      <c r="D35" s="95" t="s">
+      <c r="D35" s="82" t="s">
         <v>27</v>
       </c>
-      <c r="E35" s="95" t="s">
+      <c r="E35" s="82" t="s">
         <v>28</v>
       </c>
-      <c r="F35" s="90" t="s">
+      <c r="F35" s="80" t="s">
         <v>29</v>
       </c>
-      <c r="G35" s="95" t="s">
+      <c r="G35" s="82" t="s">
         <v>30</v>
       </c>
-      <c r="H35" s="95" t="s">
+      <c r="H35" s="82" t="s">
         <v>22</v>
       </c>
-      <c r="I35" s="96" t="s">
+      <c r="I35" s="83" t="s">
         <v>24</v>
       </c>
-      <c r="J35" s="95" t="s">
+      <c r="J35" s="82" t="s">
         <v>40</v>
       </c>
     </row>
@@ -22903,7 +22904,7 @@
         <f>(G36)/((MAX($C$36:$E$40)-MIN($C$36:$E$40)))</f>
         <v>1.3724951962668143E-4</v>
       </c>
-      <c r="I36" s="71">
+      <c r="I36" s="67">
         <f>F36-B36</f>
         <v>-1.37</v>
       </c>
@@ -22913,31 +22914,31 @@
       </c>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B37" s="109">
+      <c r="B37" s="96">
         <v>80</v>
       </c>
-      <c r="C37" s="105">
+      <c r="C37" s="92">
         <v>80.5</v>
       </c>
-      <c r="D37" s="106">
+      <c r="D37" s="93">
         <v>80.87</v>
       </c>
-      <c r="E37" s="107">
+      <c r="E37" s="94">
         <v>80.13</v>
       </c>
-      <c r="F37" s="102">
+      <c r="F37" s="89">
         <f t="shared" ref="F37" si="13">(C37+D37+E37)/3</f>
         <v>80.5</v>
       </c>
-      <c r="G37" s="102">
+      <c r="G37" s="89">
         <f t="shared" ref="G37" si="14">MAX(C37-F37,D37-F37,E37-F37)</f>
         <v>0.37000000000000455</v>
       </c>
-      <c r="H37" s="104">
+      <c r="H37" s="91">
         <f t="shared" ref="H37:H40" si="15">(G37)/((MAX($C$36:$E$40)-MIN($C$36:$E$40)))</f>
         <v>1.2695580565468176E-3</v>
       </c>
-      <c r="I37" s="110">
+      <c r="I37" s="97">
         <f>E37-B37</f>
         <v>0.12999999999999545</v>
       </c>
@@ -22968,38 +22969,38 @@
         <f t="shared" si="15"/>
         <v>7.0912251807122445E-4</v>
       </c>
-      <c r="I38" s="72">
+      <c r="I38" s="68">
         <f>F38-B38</f>
         <v>1.0933333333333337</v>
       </c>
       <c r="J38" s="47"/>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B39" s="109">
+      <c r="B39" s="96">
         <v>240</v>
       </c>
-      <c r="C39" s="105">
+      <c r="C39" s="92">
         <v>241.18</v>
       </c>
-      <c r="D39" s="106">
+      <c r="D39" s="93">
         <v>239.95</v>
       </c>
-      <c r="E39" s="111">
+      <c r="E39" s="98">
         <v>238.2</v>
       </c>
-      <c r="F39" s="102">
+      <c r="F39" s="89">
         <f t="shared" ref="F39:F40" si="16">(C39+D39+E39)/3</f>
         <v>239.77666666666664</v>
       </c>
-      <c r="G39" s="102">
+      <c r="G39" s="89">
         <f t="shared" ref="G39:G40" si="17">MAX(C39-F39,D39-F39,E39-F39)</f>
         <v>1.4033333333333644</v>
       </c>
-      <c r="H39" s="104">
+      <c r="H39" s="91">
         <f t="shared" si="15"/>
         <v>4.8151706469028426E-3</v>
       </c>
-      <c r="I39" s="112">
+      <c r="I39" s="99">
         <f>F39-B39</f>
         <v>-0.22333333333335759</v>
       </c>
@@ -23030,7 +23031,7 @@
         <f t="shared" si="15"/>
         <v>1.3267453563912163E-3</v>
       </c>
-      <c r="I40" s="73">
+      <c r="I40" s="69">
         <f>F40-B40</f>
         <v>-0.35666666666668334</v>
       </c>
@@ -23046,7 +23047,10 @@
     <mergeCell ref="B18:J18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="64" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="61" orientation="portrait" r:id="rId1"/>
+  <colBreaks count="1" manualBreakCount="1">
+    <brk id="10" max="1048575" man="1"/>
+  </colBreaks>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -23055,8 +23059,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBA93A4F-0A1B-4100-8CDC-C3CF8D673D9C}">
   <dimension ref="B1:AA40"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39:I39"/>
+    <sheetView view="pageBreakPreview" zoomScale="60" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="V20" sqref="V20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23071,60 +23075,60 @@
     <col min="8" max="8" width="18.7109375" customWidth="1"/>
     <col min="9" max="9" width="13.85546875" customWidth="1"/>
     <col min="10" max="10" width="21.28515625" customWidth="1"/>
-    <col min="11" max="11" width="17.85546875" customWidth="1"/>
+    <col min="11" max="11" width="9.5703125" customWidth="1"/>
     <col min="12" max="12" width="17.5703125" customWidth="1"/>
     <col min="13" max="13" width="19.140625" customWidth="1"/>
     <col min="14" max="14" width="19.28515625" customWidth="1"/>
     <col min="15" max="15" width="19" customWidth="1"/>
     <col min="16" max="16" width="22" customWidth="1"/>
     <col min="17" max="17" width="23.28515625" customWidth="1"/>
-    <col min="18" max="18" width="20.28515625" customWidth="1"/>
+    <col min="18" max="18" width="12" customWidth="1"/>
     <col min="19" max="19" width="29.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="85" t="s">
+      <c r="B2" s="105" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="86"/>
-      <c r="I2" s="86"/>
-      <c r="J2" s="87"/>
+      <c r="C2" s="106"/>
+      <c r="D2" s="106"/>
+      <c r="E2" s="106"/>
+      <c r="F2" s="106"/>
+      <c r="G2" s="106"/>
+      <c r="H2" s="106"/>
+      <c r="I2" s="106"/>
+      <c r="J2" s="107"/>
       <c r="S2" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="3" spans="2:27" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="88" t="s">
+      <c r="B3" s="78" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="88" t="s">
+      <c r="C3" s="78" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="88" t="s">
+      <c r="D3" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="88" t="s">
+      <c r="E3" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="89" t="s">
+      <c r="F3" s="79" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="88" t="s">
+      <c r="G3" s="78" t="s">
         <v>39</v>
       </c>
-      <c r="H3" s="88" t="s">
+      <c r="H3" s="78" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="90" t="s">
+      <c r="I3" s="80" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="89" t="s">
+      <c r="J3" s="79" t="s">
         <v>16</v>
       </c>
       <c r="L3" s="26"/>
@@ -23180,31 +23184,31 @@
       <c r="S4" s="36"/>
     </row>
     <row r="5" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="98">
+      <c r="B5" s="85">
         <v>80</v>
       </c>
-      <c r="C5" s="99">
+      <c r="C5" s="86">
         <v>21.57</v>
       </c>
-      <c r="D5" s="100">
+      <c r="D5" s="87">
         <v>21.51</v>
       </c>
-      <c r="E5" s="101">
+      <c r="E5" s="88">
         <v>21.55</v>
       </c>
-      <c r="F5" s="102">
+      <c r="F5" s="89">
         <f t="shared" ref="F5:F8" si="0">(C5+D5+E5)/3</f>
         <v>21.543333333333333</v>
       </c>
-      <c r="G5" s="103">
+      <c r="G5" s="90">
         <f t="shared" ref="G5:G8" si="1">MAX(C5-F5,D5-F5,E5-F5)*$S$3</f>
         <v>2.6666666666667282E-2</v>
       </c>
-      <c r="H5" s="104">
+      <c r="H5" s="91">
         <f t="shared" ref="H5:H8" si="2">(G5/$S$3)/(MAX($C$4:$E$10)-MIN($C$4:$E$10))</f>
         <v>4.5459711330834095E-4</v>
       </c>
-      <c r="I5" s="97" t="s">
+      <c r="I5" s="84" t="s">
         <v>38</v>
       </c>
       <c r="J5" s="47"/>
@@ -23255,27 +23259,27 @@
       <c r="S6" s="36"/>
     </row>
     <row r="7" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B7" s="98">
+      <c r="B7" s="85">
         <v>240</v>
       </c>
-      <c r="C7" s="99">
+      <c r="C7" s="86">
         <v>53.6</v>
       </c>
-      <c r="D7" s="100">
+      <c r="D7" s="87">
         <v>53.55</v>
       </c>
-      <c r="E7" s="101">
+      <c r="E7" s="88">
         <v>53.65</v>
       </c>
-      <c r="F7" s="102">
+      <c r="F7" s="89">
         <f t="shared" si="0"/>
         <v>53.6</v>
       </c>
-      <c r="G7" s="103">
+      <c r="G7" s="90">
         <f t="shared" si="1"/>
         <v>4.9999999999997158E-2</v>
       </c>
-      <c r="H7" s="104">
+      <c r="H7" s="91">
         <f t="shared" si="2"/>
         <v>8.5236958745307117E-4</v>
       </c>
@@ -23333,47 +23337,47 @@
       <c r="I9" s="36"/>
     </row>
     <row r="10" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="85" t="s">
+      <c r="B10" s="105" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="86"/>
-      <c r="D10" s="86"/>
-      <c r="E10" s="86"/>
-      <c r="F10" s="86"/>
-      <c r="G10" s="86"/>
-      <c r="H10" s="86"/>
-      <c r="I10" s="86"/>
-      <c r="J10" s="87"/>
-      <c r="Y10" s="67"/>
-      <c r="Z10" s="67"/>
-      <c r="AA10" s="67"/>
+      <c r="C10" s="106"/>
+      <c r="D10" s="106"/>
+      <c r="E10" s="106"/>
+      <c r="F10" s="106"/>
+      <c r="G10" s="106"/>
+      <c r="H10" s="106"/>
+      <c r="I10" s="106"/>
+      <c r="J10" s="107"/>
+      <c r="Y10" s="104"/>
+      <c r="Z10" s="104"/>
+      <c r="AA10" s="104"/>
     </row>
     <row r="11" spans="2:27" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="88" t="s">
+      <c r="B11" s="78" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="88" t="s">
+      <c r="C11" s="78" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="88" t="s">
+      <c r="D11" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="88" t="s">
+      <c r="E11" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="F11" s="89" t="s">
+      <c r="F11" s="79" t="s">
         <v>21</v>
       </c>
-      <c r="G11" s="88" t="s">
+      <c r="G11" s="78" t="s">
         <v>39</v>
       </c>
-      <c r="H11" s="88" t="s">
+      <c r="H11" s="78" t="s">
         <v>22</v>
       </c>
-      <c r="I11" s="90" t="s">
+      <c r="I11" s="80" t="s">
         <v>23</v>
       </c>
-      <c r="J11" s="89" t="s">
+      <c r="J11" s="79" t="s">
         <v>16</v>
       </c>
     </row>
@@ -23413,27 +23417,27 @@
       <c r="K12" s="34"/>
     </row>
     <row r="13" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B13" s="98">
+      <c r="B13" s="85">
         <v>80</v>
       </c>
-      <c r="C13" s="100">
+      <c r="C13" s="87">
         <v>25.12</v>
       </c>
-      <c r="D13" s="100">
+      <c r="D13" s="87">
         <v>24.9</v>
       </c>
-      <c r="E13" s="100">
+      <c r="E13" s="87">
         <v>25.07</v>
       </c>
-      <c r="F13" s="102">
+      <c r="F13" s="89">
         <f t="shared" ref="F13:F16" si="3">(C13+D13+E13)/3</f>
         <v>25.03</v>
       </c>
-      <c r="G13" s="103">
+      <c r="G13" s="90">
         <f t="shared" ref="G13:G16" si="4">MAX(C13-F13,D13-F13,E13-F13)*$S$3</f>
         <v>8.9999999999999858E-2</v>
       </c>
-      <c r="H13" s="104">
+      <c r="H13" s="91">
         <f t="shared" ref="H13:H16" si="5">(G13/$S$3)/(MAX($C$12:$E$16)-MIN($C$12:$E$16))</f>
         <v>1.3274336283185817E-3</v>
       </c>
@@ -23467,27 +23471,27 @@
       <c r="J14" s="47"/>
     </row>
     <row r="15" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B15" s="98">
+      <c r="B15" s="85">
         <v>240</v>
       </c>
-      <c r="C15" s="100">
+      <c r="C15" s="87">
         <v>62.43</v>
       </c>
-      <c r="D15" s="100">
+      <c r="D15" s="87">
         <v>62.09</v>
       </c>
-      <c r="E15" s="100">
+      <c r="E15" s="87">
         <v>62.14</v>
       </c>
-      <c r="F15" s="102">
+      <c r="F15" s="89">
         <f t="shared" si="3"/>
         <v>62.220000000000006</v>
       </c>
-      <c r="G15" s="103">
+      <c r="G15" s="90">
         <f t="shared" si="4"/>
         <v>0.20999999999999375</v>
       </c>
-      <c r="H15" s="104">
+      <c r="H15" s="91">
         <f t="shared" si="5"/>
         <v>3.09734513274327E-3</v>
       </c>
@@ -23523,44 +23527,44 @@
     </row>
     <row r="17" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="18" spans="2:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="91" t="s">
+      <c r="B18" s="108" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="92"/>
-      <c r="D18" s="92"/>
-      <c r="E18" s="92"/>
-      <c r="F18" s="92"/>
-      <c r="G18" s="92"/>
-      <c r="H18" s="92"/>
-      <c r="I18" s="92"/>
-      <c r="J18" s="93"/>
+      <c r="C18" s="109"/>
+      <c r="D18" s="109"/>
+      <c r="E18" s="109"/>
+      <c r="F18" s="109"/>
+      <c r="G18" s="109"/>
+      <c r="H18" s="109"/>
+      <c r="I18" s="109"/>
+      <c r="J18" s="110"/>
     </row>
     <row r="19" spans="2:15" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="94" t="s">
+      <c r="B19" s="81" t="s">
         <v>34</v>
       </c>
-      <c r="C19" s="95" t="s">
+      <c r="C19" s="82" t="s">
         <v>31</v>
       </c>
-      <c r="D19" s="95" t="s">
+      <c r="D19" s="82" t="s">
         <v>32</v>
       </c>
-      <c r="E19" s="95" t="s">
+      <c r="E19" s="82" t="s">
         <v>33</v>
       </c>
-      <c r="F19" s="90" t="s">
+      <c r="F19" s="80" t="s">
         <v>21</v>
       </c>
-      <c r="G19" s="95" t="s">
+      <c r="G19" s="82" t="s">
         <v>39</v>
       </c>
-      <c r="H19" s="95" t="s">
+      <c r="H19" s="82" t="s">
         <v>22</v>
       </c>
-      <c r="I19" s="96" t="s">
+      <c r="I19" s="83" t="s">
         <v>24</v>
       </c>
-      <c r="J19" s="95" t="s">
+      <c r="J19" s="82" t="s">
         <v>40</v>
       </c>
     </row>
@@ -23590,7 +23594,7 @@
         <f>(G20)/((MAX(C20:E24)-MIN(C20:E24)))</f>
         <v>4.0194746376811547E-3</v>
       </c>
-      <c r="I20" s="74">
+      <c r="I20" s="70">
         <f>F20-B20</f>
         <v>0</v>
       </c>
@@ -23600,32 +23604,32 @@
       </c>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B21" s="103">
+      <c r="B21" s="90">
         <f t="shared" ref="B21:B24" si="6">F5</f>
         <v>21.543333333333333</v>
       </c>
-      <c r="C21" s="100">
+      <c r="C21" s="87">
         <v>21.11</v>
       </c>
-      <c r="D21" s="100">
+      <c r="D21" s="87">
         <v>21.35</v>
       </c>
-      <c r="E21" s="100">
+      <c r="E21" s="87">
         <v>21.45</v>
       </c>
-      <c r="F21" s="102">
+      <c r="F21" s="89">
         <f t="shared" ref="F21:F24" si="7">(C21+D21+E21)/3</f>
         <v>21.303333333333331</v>
       </c>
-      <c r="G21" s="103">
+      <c r="G21" s="90">
         <f t="shared" ref="G21:G24" si="8">MAX(C21-F21,D21-F21,E21-F21)*$S$3</f>
         <v>0.14666666666666828</v>
       </c>
-      <c r="H21" s="113">
+      <c r="H21" s="100">
         <f>(G21)/((MAX(C35:E39)-MIN(C35:E39)))</f>
         <v>6.0611069785382376E-4</v>
       </c>
-      <c r="I21" s="108">
+      <c r="I21" s="95">
         <f t="shared" ref="I21:I24" si="9">F21-B21</f>
         <v>-0.24000000000000199</v>
       </c>
@@ -23658,7 +23662,7 @@
         <f>(G22)/((MAX(C39:E41)-MIN(C39:E41)))</f>
         <v>3.2507639295232545E-4</v>
       </c>
-      <c r="I22" s="75">
+      <c r="I22" s="71">
         <f t="shared" si="9"/>
         <v>0.28999999999999915</v>
       </c>
@@ -23666,32 +23670,32 @@
       <c r="L22" s="2"/>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B23" s="103">
+      <c r="B23" s="90">
         <f t="shared" si="6"/>
         <v>53.6</v>
       </c>
-      <c r="C23" s="100">
+      <c r="C23" s="87">
         <v>53.56</v>
       </c>
-      <c r="D23" s="100">
+      <c r="D23" s="87">
         <v>53.72</v>
       </c>
-      <c r="E23" s="100">
+      <c r="E23" s="87">
         <v>53.84</v>
       </c>
-      <c r="F23" s="102">
+      <c r="F23" s="89">
         <f t="shared" si="7"/>
         <v>53.706666666666671</v>
       </c>
-      <c r="G23" s="103">
+      <c r="G23" s="90">
         <f t="shared" si="8"/>
         <v>0.13333333333333286</v>
       </c>
-      <c r="H23" s="113">
+      <c r="H23" s="100">
         <f>(G23)/((MAX(C39:E41)-MIN(C39:E41)))</f>
         <v>2.600611143618742E-3</v>
       </c>
-      <c r="I23" s="108">
+      <c r="I23" s="95">
         <f t="shared" si="9"/>
         <v>0.10666666666666913</v>
       </c>
@@ -23724,7 +23728,7 @@
         <f>(G24)/((MAX(C39:E41)-MIN(C39:E41)))</f>
         <v>3.5108250438851702E-3</v>
       </c>
-      <c r="I24" s="76">
+      <c r="I24" s="72">
         <f t="shared" si="9"/>
         <v>-1.6666666666672825E-2</v>
       </c>
@@ -23735,45 +23739,45 @@
       <c r="L25" s="2"/>
     </row>
     <row r="26" spans="2:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="85" t="s">
+      <c r="B26" s="105" t="s">
         <v>35</v>
       </c>
-      <c r="C26" s="86"/>
-      <c r="D26" s="86"/>
-      <c r="E26" s="86"/>
-      <c r="F26" s="86"/>
-      <c r="G26" s="86"/>
-      <c r="H26" s="86"/>
-      <c r="I26" s="86"/>
-      <c r="J26" s="87"/>
+      <c r="C26" s="106"/>
+      <c r="D26" s="106"/>
+      <c r="E26" s="106"/>
+      <c r="F26" s="106"/>
+      <c r="G26" s="106"/>
+      <c r="H26" s="106"/>
+      <c r="I26" s="106"/>
+      <c r="J26" s="107"/>
       <c r="L26" s="2"/>
     </row>
     <row r="27" spans="2:15" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="88" t="s">
+      <c r="B27" s="78" t="s">
         <v>15</v>
       </c>
-      <c r="C27" s="88" t="s">
+      <c r="C27" s="78" t="s">
         <v>12</v>
       </c>
-      <c r="D27" s="88" t="s">
+      <c r="D27" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="E27" s="88" t="s">
+      <c r="E27" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="F27" s="89" t="s">
+      <c r="F27" s="79" t="s">
         <v>21</v>
       </c>
-      <c r="G27" s="88" t="s">
+      <c r="G27" s="78" t="s">
         <v>39</v>
       </c>
-      <c r="H27" s="88" t="s">
+      <c r="H27" s="78" t="s">
         <v>22</v>
       </c>
-      <c r="I27" s="90" t="s">
+      <c r="I27" s="80" t="s">
         <v>23</v>
       </c>
-      <c r="J27" s="89" t="s">
+      <c r="J27" s="79" t="s">
         <v>16</v>
       </c>
       <c r="L27" s="2"/>
@@ -23814,27 +23818,27 @@
       <c r="L28" s="2"/>
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B29" s="98">
+      <c r="B29" s="85">
         <v>80</v>
       </c>
-      <c r="C29" s="100">
+      <c r="C29" s="87">
         <v>21.11</v>
       </c>
-      <c r="D29" s="100">
+      <c r="D29" s="87">
         <v>21.35</v>
       </c>
-      <c r="E29" s="100">
+      <c r="E29" s="87">
         <v>21.45</v>
       </c>
-      <c r="F29" s="102">
+      <c r="F29" s="89">
         <f t="shared" ref="F29:F32" si="10">(C29+D29+E29)/3</f>
         <v>21.303333333333331</v>
       </c>
-      <c r="G29" s="103">
+      <c r="G29" s="90">
         <f t="shared" ref="G29:G32" si="11">MAX(C29-F29,D29-F29,E29-F29)*$S$3</f>
         <v>0.14666666666666828</v>
       </c>
-      <c r="H29" s="104">
+      <c r="H29" s="91">
         <f>(G29/$S$3)/(MAX($C$28:$E$32)-MIN($C$28:$E$32))</f>
         <v>2.4909420289855348E-3</v>
       </c>
@@ -23874,27 +23878,27 @@
       <c r="O30" s="42"/>
     </row>
     <row r="31" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B31" s="98">
+      <c r="B31" s="85">
         <v>240</v>
       </c>
-      <c r="C31" s="100">
+      <c r="C31" s="87">
         <v>53.56</v>
       </c>
-      <c r="D31" s="100">
+      <c r="D31" s="87">
         <v>53.72</v>
       </c>
-      <c r="E31" s="100">
+      <c r="E31" s="87">
         <v>53.84</v>
       </c>
-      <c r="F31" s="102">
+      <c r="F31" s="89">
         <f t="shared" si="10"/>
         <v>53.706666666666671</v>
       </c>
-      <c r="G31" s="103">
+      <c r="G31" s="90">
         <f t="shared" si="11"/>
         <v>0.13333333333333286</v>
       </c>
-      <c r="H31" s="104">
+      <c r="H31" s="91">
         <f t="shared" si="12"/>
         <v>2.2644927536231807E-3</v>
       </c>
@@ -23933,44 +23937,44 @@
       <c r="G33"/>
     </row>
     <row r="34" spans="2:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="91" t="s">
+      <c r="B34" s="108" t="s">
         <v>25</v>
       </c>
-      <c r="C34" s="92"/>
-      <c r="D34" s="92"/>
-      <c r="E34" s="92"/>
-      <c r="F34" s="92"/>
-      <c r="G34" s="92"/>
-      <c r="H34" s="92"/>
-      <c r="I34" s="92"/>
-      <c r="J34" s="93"/>
+      <c r="C34" s="109"/>
+      <c r="D34" s="109"/>
+      <c r="E34" s="109"/>
+      <c r="F34" s="109"/>
+      <c r="G34" s="109"/>
+      <c r="H34" s="109"/>
+      <c r="I34" s="109"/>
+      <c r="J34" s="110"/>
     </row>
     <row r="35" spans="2:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="94" t="s">
+      <c r="B35" s="81" t="s">
         <v>15</v>
       </c>
-      <c r="C35" s="95" t="s">
+      <c r="C35" s="82" t="s">
         <v>26</v>
       </c>
-      <c r="D35" s="95" t="s">
+      <c r="D35" s="82" t="s">
         <v>27</v>
       </c>
-      <c r="E35" s="95" t="s">
+      <c r="E35" s="82" t="s">
         <v>28</v>
       </c>
-      <c r="F35" s="90" t="s">
+      <c r="F35" s="80" t="s">
         <v>29</v>
       </c>
-      <c r="G35" s="95" t="s">
+      <c r="G35" s="82" t="s">
         <v>30</v>
       </c>
-      <c r="H35" s="95" t="s">
+      <c r="H35" s="82" t="s">
         <v>22</v>
       </c>
-      <c r="I35" s="96" t="s">
+      <c r="I35" s="83" t="s">
         <v>24</v>
       </c>
-      <c r="J35" s="95" t="s">
+      <c r="J35" s="82" t="s">
         <v>40</v>
       </c>
     </row>
@@ -23999,7 +24003,7 @@
         <f>(G36)/((MAX($C$36:$E$40)-MIN($C$36:$E$40)))</f>
         <v>3.5390551864283002E-4</v>
       </c>
-      <c r="I36" s="74">
+      <c r="I36" s="70">
         <f>F36-B36</f>
         <v>-1.1333333333333335</v>
       </c>
@@ -24009,31 +24013,31 @@
       </c>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B37" s="109">
+      <c r="B37" s="96">
         <v>80</v>
       </c>
-      <c r="C37" s="105">
+      <c r="C37" s="92">
         <v>80.45</v>
       </c>
-      <c r="D37" s="106">
+      <c r="D37" s="93">
         <v>80.290000000000006</v>
       </c>
-      <c r="E37" s="107">
+      <c r="E37" s="94">
         <v>80.25</v>
       </c>
-      <c r="F37" s="102">
+      <c r="F37" s="89">
         <f t="shared" ref="F37:F39" si="13">(C37+D37+E37)/3</f>
         <v>80.33</v>
       </c>
-      <c r="G37" s="102">
+      <c r="G37" s="89">
         <f t="shared" ref="G37:G39" si="14">MAX(C37-F37,D37-F37,E37-F37)</f>
         <v>0.12000000000000455</v>
       </c>
-      <c r="H37" s="104">
+      <c r="H37" s="91">
         <f t="shared" ref="H37:H39" si="15">(G37)/((MAX($C$36:$E$40)-MIN($C$36:$E$40)))</f>
         <v>4.1098705390781753E-4</v>
       </c>
-      <c r="I37" s="108">
+      <c r="I37" s="95">
         <f t="shared" ref="I37:I40" si="16">F37-B37</f>
         <v>0.32999999999999829</v>
       </c>
@@ -24064,38 +24068,38 @@
         <f t="shared" si="15"/>
         <v>2.4773386304997921E-3</v>
       </c>
-      <c r="I38" s="75">
+      <c r="I38" s="71">
         <f t="shared" si="16"/>
         <v>1.2066666666666777</v>
       </c>
       <c r="J38" s="47"/>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B39" s="109">
+      <c r="B39" s="96">
         <v>240</v>
       </c>
-      <c r="C39" s="105">
+      <c r="C39" s="92">
         <v>239.43</v>
       </c>
-      <c r="D39" s="106">
+      <c r="D39" s="93">
         <v>240.65</v>
       </c>
-      <c r="E39" s="107">
+      <c r="E39" s="94">
         <v>240.7</v>
       </c>
-      <c r="F39" s="102">
+      <c r="F39" s="89">
         <f t="shared" si="13"/>
         <v>240.26</v>
       </c>
-      <c r="G39" s="102">
+      <c r="G39" s="89">
         <f t="shared" si="14"/>
         <v>0.43999999999999773</v>
       </c>
-      <c r="H39" s="104">
+      <c r="H39" s="91">
         <f t="shared" si="15"/>
         <v>1.506952530995266E-3</v>
       </c>
-      <c r="I39" s="108">
+      <c r="I39" s="95">
         <f t="shared" si="16"/>
         <v>0.25999999999999091</v>
       </c>
@@ -24126,7 +24130,7 @@
         <f>(G40)/((MAX($C$36:$E$40)-MIN($C$36:$E$40)))</f>
         <v>1.9864374272207936E-3</v>
       </c>
-      <c r="I40" s="76">
+      <c r="I40" s="72">
         <f t="shared" si="16"/>
         <v>0.12000000000006139</v>
       </c>
@@ -24142,7 +24146,10 @@
     <mergeCell ref="B18:J18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="64" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="61" orientation="portrait" r:id="rId1"/>
+  <colBreaks count="1" manualBreakCount="1">
+    <brk id="10" max="39" man="1"/>
+  </colBreaks>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -24151,8 +24158,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99EB5308-17EB-475C-A711-221EA997DC89}">
   <dimension ref="B1:AA40"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34:J35"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection sqref="A1:R1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24167,60 +24174,60 @@
     <col min="8" max="8" width="18.7109375" customWidth="1"/>
     <col min="9" max="9" width="13.85546875" customWidth="1"/>
     <col min="10" max="10" width="21.28515625" customWidth="1"/>
-    <col min="11" max="11" width="17.85546875" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" customWidth="1"/>
     <col min="12" max="12" width="17.5703125" customWidth="1"/>
     <col min="13" max="13" width="19.140625" customWidth="1"/>
     <col min="14" max="14" width="19.28515625" customWidth="1"/>
     <col min="15" max="15" width="19" customWidth="1"/>
     <col min="16" max="16" width="22" customWidth="1"/>
     <col min="17" max="17" width="23.28515625" customWidth="1"/>
-    <col min="18" max="18" width="20.28515625" customWidth="1"/>
+    <col min="18" max="18" width="14.140625" customWidth="1"/>
     <col min="19" max="19" width="29.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="85" t="s">
+      <c r="B2" s="105" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="86"/>
-      <c r="I2" s="86"/>
-      <c r="J2" s="87"/>
+      <c r="C2" s="106"/>
+      <c r="D2" s="106"/>
+      <c r="E2" s="106"/>
+      <c r="F2" s="106"/>
+      <c r="G2" s="106"/>
+      <c r="H2" s="106"/>
+      <c r="I2" s="106"/>
+      <c r="J2" s="107"/>
       <c r="S2" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="3" spans="2:27" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="88" t="s">
+      <c r="B3" s="78" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="88" t="s">
+      <c r="C3" s="78" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="88" t="s">
+      <c r="D3" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="88" t="s">
+      <c r="E3" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="89" t="s">
+      <c r="F3" s="79" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="88" t="s">
+      <c r="G3" s="78" t="s">
         <v>39</v>
       </c>
-      <c r="H3" s="88" t="s">
+      <c r="H3" s="78" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="90" t="s">
+      <c r="I3" s="80" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="89" t="s">
+      <c r="J3" s="79" t="s">
         <v>16</v>
       </c>
       <c r="L3" s="26"/>
@@ -24300,7 +24307,7 @@
         <f t="shared" ref="H5:H8" si="2">(G5/$S$3)/(MAX($C$4:$E$10)-MIN($C$4:$E$10))</f>
         <v>4.1838606143971089E-3</v>
       </c>
-      <c r="I5" s="97" t="s">
+      <c r="I5" s="84" t="s">
         <v>38</v>
       </c>
       <c r="J5" s="47"/>
@@ -24429,47 +24436,47 @@
       <c r="I9" s="36"/>
     </row>
     <row r="10" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="85" t="s">
+      <c r="B10" s="105" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="86"/>
-      <c r="D10" s="86"/>
-      <c r="E10" s="86"/>
-      <c r="F10" s="86"/>
-      <c r="G10" s="86"/>
-      <c r="H10" s="86"/>
-      <c r="I10" s="86"/>
-      <c r="J10" s="87"/>
-      <c r="Y10" s="67"/>
-      <c r="Z10" s="67"/>
-      <c r="AA10" s="67"/>
+      <c r="C10" s="106"/>
+      <c r="D10" s="106"/>
+      <c r="E10" s="106"/>
+      <c r="F10" s="106"/>
+      <c r="G10" s="106"/>
+      <c r="H10" s="106"/>
+      <c r="I10" s="106"/>
+      <c r="J10" s="107"/>
+      <c r="Y10" s="104"/>
+      <c r="Z10" s="104"/>
+      <c r="AA10" s="104"/>
     </row>
     <row r="11" spans="2:27" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="88" t="s">
+      <c r="B11" s="78" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="88" t="s">
+      <c r="C11" s="78" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="88" t="s">
+      <c r="D11" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="88" t="s">
+      <c r="E11" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="F11" s="89" t="s">
+      <c r="F11" s="79" t="s">
         <v>21</v>
       </c>
-      <c r="G11" s="88" t="s">
+      <c r="G11" s="78" t="s">
         <v>39</v>
       </c>
-      <c r="H11" s="88" t="s">
+      <c r="H11" s="78" t="s">
         <v>22</v>
       </c>
-      <c r="I11" s="90" t="s">
+      <c r="I11" s="80" t="s">
         <v>23</v>
       </c>
-      <c r="J11" s="89" t="s">
+      <c r="J11" s="79" t="s">
         <v>16</v>
       </c>
     </row>
@@ -24619,44 +24626,44 @@
     </row>
     <row r="17" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="18" spans="2:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="91" t="s">
+      <c r="B18" s="108" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="92"/>
-      <c r="D18" s="92"/>
-      <c r="E18" s="92"/>
-      <c r="F18" s="92"/>
-      <c r="G18" s="92"/>
-      <c r="H18" s="92"/>
-      <c r="I18" s="92"/>
-      <c r="J18" s="93"/>
+      <c r="C18" s="109"/>
+      <c r="D18" s="109"/>
+      <c r="E18" s="109"/>
+      <c r="F18" s="109"/>
+      <c r="G18" s="109"/>
+      <c r="H18" s="109"/>
+      <c r="I18" s="109"/>
+      <c r="J18" s="110"/>
     </row>
     <row r="19" spans="2:15" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="94" t="s">
+      <c r="B19" s="81" t="s">
         <v>34</v>
       </c>
-      <c r="C19" s="95" t="s">
+      <c r="C19" s="82" t="s">
         <v>31</v>
       </c>
-      <c r="D19" s="95" t="s">
+      <c r="D19" s="82" t="s">
         <v>32</v>
       </c>
-      <c r="E19" s="95" t="s">
+      <c r="E19" s="82" t="s">
         <v>33</v>
       </c>
-      <c r="F19" s="90" t="s">
+      <c r="F19" s="80" t="s">
         <v>21</v>
       </c>
-      <c r="G19" s="95" t="s">
+      <c r="G19" s="82" t="s">
         <v>39</v>
       </c>
-      <c r="H19" s="95" t="s">
+      <c r="H19" s="82" t="s">
         <v>22</v>
       </c>
-      <c r="I19" s="96" t="s">
+      <c r="I19" s="83" t="s">
         <v>24</v>
       </c>
-      <c r="J19" s="95" t="s">
+      <c r="J19" s="82" t="s">
         <v>40</v>
       </c>
     </row>
@@ -24686,7 +24693,7 @@
         <f>(G20)/((MAX($C$20:$E$24)-MIN($C$20:$E$24)))</f>
         <v>3.1419594401599512E-3</v>
       </c>
-      <c r="I20" s="74">
+      <c r="I20" s="70">
         <f>F20-B20</f>
         <v>-0.1333333333333333</v>
       </c>
@@ -24721,7 +24728,7 @@
         <f t="shared" ref="H21:H24" si="8">(G21)/((MAX($C$20:$E$24)-MIN($C$20:$E$24)))</f>
         <v>1.999428734647252E-3</v>
       </c>
-      <c r="I21" s="75">
+      <c r="I21" s="71">
         <f t="shared" ref="I21:I24" si="9">F21-B21</f>
         <v>6.6666666666669983E-2</v>
       </c>
@@ -24747,14 +24754,14 @@
         <v>35.323333333333331</v>
       </c>
       <c r="G22" s="56">
-        <f t="shared" ref="G21:G24" si="10">MAX(C22-F22,D22-F22,E22-F22)*$S$3</f>
+        <f t="shared" ref="G22:G24" si="10">MAX(C22-F22,D22-F22,E22-F22)*$S$3</f>
         <v>1.6666666666672825E-2</v>
       </c>
       <c r="H22" s="60">
         <f t="shared" si="8"/>
         <v>2.8563267637828321E-4</v>
       </c>
-      <c r="I22" s="75">
+      <c r="I22" s="71">
         <f t="shared" si="9"/>
         <v>0.11333333333332973</v>
       </c>
@@ -24787,7 +24794,7 @@
         <f t="shared" si="8"/>
         <v>2.8563267637816145E-4</v>
       </c>
-      <c r="I23" s="75">
+      <c r="I23" s="71">
         <f t="shared" si="9"/>
         <v>-3.9999999999999147E-2</v>
       </c>
@@ -24820,7 +24827,7 @@
         <f t="shared" si="8"/>
         <v>4.2273636103970814E-3</v>
       </c>
-      <c r="I24" s="76">
+      <c r="I24" s="72">
         <f t="shared" si="9"/>
         <v>-5.0000000000004263E-2</v>
       </c>
@@ -24831,45 +24838,45 @@
       <c r="L25" s="2"/>
     </row>
     <row r="26" spans="2:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="85" t="s">
+      <c r="B26" s="105" t="s">
         <v>35</v>
       </c>
-      <c r="C26" s="86"/>
-      <c r="D26" s="86"/>
-      <c r="E26" s="86"/>
-      <c r="F26" s="86"/>
-      <c r="G26" s="86"/>
-      <c r="H26" s="86"/>
-      <c r="I26" s="86"/>
-      <c r="J26" s="87"/>
+      <c r="C26" s="106"/>
+      <c r="D26" s="106"/>
+      <c r="E26" s="106"/>
+      <c r="F26" s="106"/>
+      <c r="G26" s="106"/>
+      <c r="H26" s="106"/>
+      <c r="I26" s="106"/>
+      <c r="J26" s="107"/>
       <c r="L26" s="2"/>
     </row>
     <row r="27" spans="2:15" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="88" t="s">
+      <c r="B27" s="78" t="s">
         <v>15</v>
       </c>
-      <c r="C27" s="88" t="s">
+      <c r="C27" s="78" t="s">
         <v>12</v>
       </c>
-      <c r="D27" s="88" t="s">
+      <c r="D27" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="E27" s="88" t="s">
+      <c r="E27" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="F27" s="89" t="s">
+      <c r="F27" s="79" t="s">
         <v>21</v>
       </c>
-      <c r="G27" s="88" t="s">
+      <c r="G27" s="78" t="s">
         <v>39</v>
       </c>
-      <c r="H27" s="88" t="s">
+      <c r="H27" s="78" t="s">
         <v>22</v>
       </c>
-      <c r="I27" s="90" t="s">
+      <c r="I27" s="80" t="s">
         <v>23</v>
       </c>
-      <c r="J27" s="89" t="s">
+      <c r="J27" s="79" t="s">
         <v>16</v>
       </c>
       <c r="L27" s="2"/>
@@ -25029,44 +25036,44 @@
       <c r="G33"/>
     </row>
     <row r="34" spans="2:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="91" t="s">
+      <c r="B34" s="108" t="s">
         <v>25</v>
       </c>
-      <c r="C34" s="92"/>
-      <c r="D34" s="92"/>
-      <c r="E34" s="92"/>
-      <c r="F34" s="92"/>
-      <c r="G34" s="92"/>
-      <c r="H34" s="92"/>
-      <c r="I34" s="92"/>
-      <c r="J34" s="93"/>
+      <c r="C34" s="109"/>
+      <c r="D34" s="109"/>
+      <c r="E34" s="109"/>
+      <c r="F34" s="109"/>
+      <c r="G34" s="109"/>
+      <c r="H34" s="109"/>
+      <c r="I34" s="109"/>
+      <c r="J34" s="110"/>
     </row>
     <row r="35" spans="2:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="94" t="s">
+      <c r="B35" s="81" t="s">
         <v>15</v>
       </c>
-      <c r="C35" s="95" t="s">
+      <c r="C35" s="82" t="s">
         <v>26</v>
       </c>
-      <c r="D35" s="95" t="s">
+      <c r="D35" s="82" t="s">
         <v>27</v>
       </c>
-      <c r="E35" s="95" t="s">
+      <c r="E35" s="82" t="s">
         <v>28</v>
       </c>
-      <c r="F35" s="90" t="s">
+      <c r="F35" s="80" t="s">
         <v>29</v>
       </c>
-      <c r="G35" s="95" t="s">
+      <c r="G35" s="82" t="s">
         <v>30</v>
       </c>
-      <c r="H35" s="95" t="s">
+      <c r="H35" s="82" t="s">
         <v>22</v>
       </c>
-      <c r="I35" s="96" t="s">
+      <c r="I35" s="83" t="s">
         <v>24</v>
       </c>
-      <c r="J35" s="95" t="s">
+      <c r="J35" s="82" t="s">
         <v>40</v>
       </c>
     </row>
@@ -25095,7 +25102,7 @@
         <f>(G36)/((MAX($C$36:$E$40)-MIN($C$36:$E$40)))</f>
         <v>1.1102336068857376E-3</v>
       </c>
-      <c r="I36" s="74">
+      <c r="I36" s="70">
         <f>F36-B36</f>
         <v>-1.1433333333333333</v>
       </c>
@@ -25129,7 +25136,7 @@
         <f t="shared" ref="H37:H39" si="16">(G37)/((MAX($C$36:$E$40)-MIN($C$36:$E$40)))</f>
         <v>1.6825189712598601E-3</v>
       </c>
-      <c r="I37" s="75">
+      <c r="I37" s="71">
         <f t="shared" ref="I37:I40" si="17">F37-B37</f>
         <v>0.15999999999999659</v>
       </c>
@@ -25160,7 +25167,7 @@
         <f t="shared" si="16"/>
         <v>7.7830809554873962E-4</v>
       </c>
-      <c r="I38" s="75">
+      <c r="I38" s="71">
         <f t="shared" si="17"/>
         <v>1.3133333333333326</v>
       </c>
@@ -25191,7 +25198,7 @@
         <f t="shared" si="16"/>
         <v>1.453604825510139E-3</v>
       </c>
-      <c r="I39" s="75">
+      <c r="I39" s="71">
         <f t="shared" si="17"/>
         <v>-4.3333333333322344E-2</v>
       </c>
@@ -25222,7 +25229,7 @@
         <f>(G40)/((MAX($C$36:$E$40)-MIN($C$36:$E$40)))</f>
         <v>1.6138447275348363E-3</v>
       </c>
-      <c r="I40" s="76">
+      <c r="I40" s="72">
         <f t="shared" si="17"/>
         <v>-0.77999999999997272</v>
       </c>
@@ -25238,7 +25245,10 @@
     <mergeCell ref="B18:J18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="64" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="61" orientation="portrait" r:id="rId1"/>
+  <colBreaks count="1" manualBreakCount="1">
+    <brk id="10" max="39" man="1"/>
+  </colBreaks>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -25263,15 +25273,15 @@
   <sheetData>
     <row r="1" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="68" t="s">
+      <c r="B2" s="111" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
-      <c r="G2" s="69"/>
-      <c r="H2" s="70"/>
+      <c r="C2" s="112"/>
+      <c r="D2" s="112"/>
+      <c r="E2" s="112"/>
+      <c r="F2" s="112"/>
+      <c r="G2" s="112"/>
+      <c r="H2" s="113"/>
     </row>
     <row r="3" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="23" t="s">
@@ -25589,15 +25599,15 @@
       <c r="F16" s="1"/>
     </row>
     <row r="17" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="68" t="s">
+      <c r="B17" s="111" t="s">
         <v>2</v>
       </c>
-      <c r="C17" s="69"/>
-      <c r="D17" s="69"/>
-      <c r="E17" s="69"/>
-      <c r="F17" s="69"/>
-      <c r="G17" s="69"/>
-      <c r="H17" s="70"/>
+      <c r="C17" s="112"/>
+      <c r="D17" s="112"/>
+      <c r="E17" s="112"/>
+      <c r="F17" s="112"/>
+      <c r="G17" s="112"/>
+      <c r="H17" s="113"/>
     </row>
     <row r="18" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="23" t="s">
@@ -25919,6 +25929,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c0c8a948-a8a2-431d-a436-e17f069363af">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="6b745cbd-a34e-432a-9900-41e3803aa2e9" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100FD8BE65C2F837343AC2660C8B0889EAE" ma:contentTypeVersion="14" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="b7eb9a75dd4706810b4c69081d8d48fe">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c0c8a948-a8a2-431d-a436-e17f069363af" xmlns:ns3="6b745cbd-a34e-432a-9900-41e3803aa2e9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f5420ca96eed7fa2cb1a1994b234afa6" ns2:_="" ns3:_="">
     <xsd:import namespace="c0c8a948-a8a2-431d-a436-e17f069363af"/>
@@ -26149,17 +26170,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c0c8a948-a8a2-431d-a436-e17f069363af">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="6b745cbd-a34e-432a-9900-41e3803aa2e9" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -26170,6 +26180,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AF9C1C43-49EE-494C-B635-B785FB629686}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="6b745cbd-a34e-432a-9900-41e3803aa2e9"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="c0c8a948-a8a2-431d-a436-e17f069363af"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A5FF9E8C-A979-49D8-B0D6-7BF035D44D87}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -26188,23 +26215,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AF9C1C43-49EE-494C-B635-B785FB629686}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="c0c8a948-a8a2-431d-a436-e17f069363af"/>
-    <ds:schemaRef ds:uri="6b745cbd-a34e-432a-9900-41e3803aa2e9"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E33CB14B-EEEA-4E1E-B623-D870A775B6DB}">
   <ds:schemaRefs>

</xml_diff>